<commit_message>
added metadata files and deleted duplicate fastq file
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_H.BROWN_09.24.20.xlsx
+++ b/bioSample/bioSample_H.BROWN_09.24.20.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB036E6E-E484-7444-B628-1032FF4F6949}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A13707-7190-7C48-B5EF-24A8553C9730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="1520" windowWidth="23060" windowHeight="15000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10540" yWindow="1520" windowWidth="23060" windowHeight="15000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -183,9 +183,6 @@
     <t>TDY2261</t>
   </si>
   <si>
-    <t>TDY22744</t>
-  </si>
-  <si>
     <t>CNAG_02700</t>
   </si>
   <si>
@@ -205,6 +202,9 @@
   </si>
   <si>
     <t>CNAG_00883</t>
+  </si>
+  <si>
+    <t>TDY2274</t>
   </si>
 </sst>
 </file>
@@ -559,7 +559,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A25"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,7 +673,7 @@
         <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
@@ -702,7 +702,7 @@
         <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G5" t="s">
         <v>13</v>
@@ -934,7 +934,7 @@
         <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
         <v>13</v>
@@ -1166,7 +1166,7 @@
         <v>49</v>
       </c>
       <c r="F21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G21" t="s">
         <v>13</v>
@@ -1195,7 +1195,7 @@
         <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G22" t="s">
         <v>13</v>
@@ -1224,7 +1224,7 @@
         <v>51</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G23" t="s">
         <v>13</v>
@@ -1279,10 +1279,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" t="s">
         <v>52</v>
-      </c>
-      <c r="F25" t="s">
-        <v>53</v>
       </c>
       <c r="G25" t="s">
         <v>13</v>

</xml_diff>